<commit_message>
change Guid on int
</commit_message>
<xml_diff>
--- a/Db.xlsx
+++ b/Db.xlsx
@@ -212,12 +212,6 @@
     <t>SubId?</t>
   </si>
   <si>
-    <t>IdGym?</t>
-  </si>
-  <si>
-    <t>IdTrMach?</t>
-  </si>
-  <si>
     <t>PosId?</t>
   </si>
   <si>
@@ -252,6 +246,12 @@
   </si>
   <si>
     <t>PosId</t>
+  </si>
+  <si>
+    <t>TrMachId?</t>
+  </si>
+  <si>
+    <t>Time</t>
   </si>
 </sst>
 </file>
@@ -1269,7 +1269,7 @@
   <dimension ref="A1:R26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R9" sqref="R9"/>
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1311,7 +1311,7 @@
     </row>
     <row r="2" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>0</v>
@@ -1326,10 +1326,10 @@
         <v>61</v>
       </c>
       <c r="J2" s="20" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="K2" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L2" s="21" t="s">
         <v>0</v>
@@ -1341,10 +1341,10 @@
         <v>12</v>
       </c>
       <c r="O2" s="22" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Q2" s="39" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="R2" s="40" t="s">
         <v>0</v>
@@ -1567,13 +1567,13 @@
       </c>
       <c r="H11" s="121"/>
       <c r="J11" s="24" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="K11" s="25" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L11" s="26" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1587,10 +1587,10 @@
         <v>28</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="J12" s="59">
         <v>1</v>
@@ -1701,19 +1701,19 @@
         <v>2</v>
       </c>
       <c r="J17" s="29" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="K17" s="30" t="s">
         <v>0</v>
       </c>
       <c r="L17" s="30" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="M17" s="31" t="s">
         <v>45</v>
       </c>
       <c r="O17" s="37" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="P17" s="38" t="s">
         <v>0</v>
@@ -1835,7 +1835,7 @@
     </row>
     <row r="23" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="J23" s="34" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K23" s="35" t="s">
         <v>0</v>
@@ -1844,7 +1844,7 @@
         <v>50</v>
       </c>
       <c r="M23" s="36" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.3">
@@ -1858,7 +1858,7 @@
         <v>54</v>
       </c>
       <c r="M24" s="72">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.3">
@@ -1872,7 +1872,7 @@
         <v>55</v>
       </c>
       <c r="M25" s="74">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>